<commit_message>
� ix: Configure migration routes and organization
</commit_message>
<xml_diff>
--- a/src/templates/formato_certificado_estandar.xlsx
+++ b/src/templates/formato_certificado_estandar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvan.sanabria\OneDrive - Servimeters\Documentos\Software\consulta_certificados\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7010B33-AA65-4D68-B55E-D2FEE9B6A29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877F5B5F-2FCD-42C2-930D-0073A15E86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
+    <workbookView xWindow="35460" yWindow="1860" windowWidth="21585" windowHeight="10605" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>CÓDIGO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -47,19 +44,13 @@
     <t xml:space="preserve">CAPACITACION </t>
   </si>
   <si>
-    <t>FECHA</t>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>ALBA AIDEE AGUILAR ABREGO</t>
   </si>
   <si>
     <t>AUDITOR INTERNO DE SISTEMAS DE GESTIÓN DE LA CALIDAD SEGÚN LA NORMA ISO 9001:2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ALBA AIDEE AGUILAR ABREGO</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>#2AB0AMGGPN2@M0X1</t>
   </si>
   <si>
     <t>https://servimeters-my.sharepoint.com/:x:/r/personal/duvan_sanabria_servimeters_com/_layouts/15/Doc.aspx?sourcedoc=%7B9D631C9C-C83D-4260-8520-0BA5934135E4%7D&amp;file=Prog%20en%20Sitio-RICARDO.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1</t>
@@ -113,14 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -436,66 +423,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED78EBC-390D-4A45-8A90-C0D493A75DE1}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38" style="4" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" customWidth="1"/>
+    <col min="3" max="3" width="38" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>45252</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>78787</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{88725C7D-AE38-4FB1-9A09-0E7D09D6C780}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{48F0C3E7-005F-435C-B792-313DD22A3626}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: querying certificates, validating the country type of the record and improving views
</commit_message>
<xml_diff>
--- a/src/templates/formato_certificado_estandar.xlsx
+++ b/src/templates/formato_certificado_estandar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvan.sanabria\OneDrive - Servimeters\Documentos\Software\consulta_certificados\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servimeters-my.sharepoint.com/personal/duvan_sanabria_servimeters_com/Documents/Documentos/Software/consulta_certificados/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877F5B5F-2FCD-42C2-930D-0073A15E86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{877F5B5F-2FCD-42C2-930D-0073A15E86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E76D7C9-7714-4B39-86DC-F59120C49FC1}"/>
   <bookViews>
-    <workbookView xWindow="35460" yWindow="1860" windowWidth="21585" windowHeight="10605" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>https://servimeters-my.sharepoint.com/:x:/r/personal/duvan_sanabria_servimeters_com/_layouts/15/Doc.aspx?sourcedoc=%7B9D631C9C-C83D-4260-8520-0BA5934135E4%7D&amp;file=Prog%20en%20Sitio-RICARDO.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Colombia</t>
   </si>
 </sst>
 </file>
@@ -423,20 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED78EBC-390D-4A45-8A90-C0D493A75DE1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="90.140625" customWidth="1"/>
-    <col min="3" max="3" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +455,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -457,8 +469,11 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -468,8 +483,11 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -479,8 +497,11 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -489,6 +510,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add country column when inserting certificates
</commit_message>
<xml_diff>
--- a/src/templates/formato_certificado_estandar.xlsx
+++ b/src/templates/formato_certificado_estandar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servimeters-my.sharepoint.com/personal/duvan_sanabria_servimeters_com/Documents/Documentos/Software/consulta_certificados/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{877F5B5F-2FCD-42C2-930D-0073A15E86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E76D7C9-7714-4B39-86DC-F59120C49FC1}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{877F5B5F-2FCD-42C2-930D-0073A15E86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B8B7887-0340-4E15-8C22-6DCECE27BBE1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{627C57AE-B618-423A-8333-07391A41D1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -47,9 +47,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>ALBA AIDEE AGUILAR ABREGO</t>
-  </si>
-  <si>
     <t>AUDITOR INTERNO DE SISTEMAS DE GESTIÓN DE LA CALIDAD SEGÚN LA NORMA ISO 9001:2015</t>
   </si>
   <si>
@@ -59,10 +56,10 @@
     <t>Pais</t>
   </si>
   <si>
-    <t>Panama</t>
-  </si>
-  <si>
     <t>Colombia</t>
+  </si>
+  <si>
+    <t>Duvan Camilo</t>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,63 +453,63 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>